<commit_message>
update import product  xx
</commit_message>
<xml_diff>
--- a/Winform/SaleManager/SaleManager/Requiment/temp.xlsx
+++ b/Winform/SaleManager/SaleManager/Requiment/temp.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguyen-trong-hung\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\H\Angular\SaleManager\Winform\SaleManager\SaleManager\Requiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4B194F-B630-408F-AA4C-EFB426698038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Barcode</t>
   </si>
@@ -42,9 +43,6 @@
     <t>Giá bán</t>
   </si>
   <si>
-    <t>Hsd(tháng)</t>
-  </si>
-  <si>
     <t>Hsd</t>
   </si>
   <si>
@@ -57,22 +55,10 @@
     <t>Dầu ăn simply 2l</t>
   </si>
   <si>
-    <t>chai</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Thuỷ(bibica)</t>
-  </si>
-  <si>
     <t>3110354325000</t>
   </si>
   <si>
     <t>Thuốc lá Thăng Long</t>
-  </si>
-  <si>
-    <t>cây</t>
-  </si>
-  <si>
-    <t>Nguyễn Đức Cảnh(ĐL cấp 1)</t>
   </si>
   <si>
     <r>
@@ -124,12 +110,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="#,###"/>
-    <numFmt numFmtId="177" formatCode="#"/>
-    <numFmt numFmtId="178" formatCode="#0.0"/>
-    <numFmt numFmtId="179" formatCode="dd/mm/yyyy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="177" formatCode="0.0_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0_);[Red]\(#,##0\)"/>
+    <numFmt numFmtId="179" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -162,7 +147,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,22 +170,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -514,190 +522,161 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="R1" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="C2" s="12">
         <v>1300000</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="16">
         <v>10</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="12">
         <f>ROUND(C2/D2,1)</f>
         <v>130000</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="14">
+        <v>140000</v>
+      </c>
+      <c r="H2" s="19">
+        <v>44184</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="3"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4">
-        <v>140000</v>
-      </c>
-      <c r="H2" s="6">
-        <v>24</v>
-      </c>
-      <c r="I2" s="7">
-        <f ca="1">IF(H2&lt;1, NOW()+30*H2, EDATE(NOW(),H2))</f>
-        <v>44910</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="C3" s="12">
         <v>750000</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="16">
         <v>10</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="12">
         <f>ROUND(C3/D3,1)</f>
         <v>75000</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="4">
+      <c r="F3" s="3"/>
+      <c r="G3" s="14">
         <v>80000</v>
       </c>
-      <c r="H3" s="6">
-        <v>40</v>
-      </c>
-      <c r="I3" s="7">
-        <f ca="1">IF(H3&lt;1, NOW()+30*H3, EDATE(NOW(),H3))</f>
-        <v>45397</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="3"/>
+      <c r="H3" s="19">
+        <v>44184</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="2"/>
       <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
+      <c r="P3" s="2"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
+      <c r="R3" s="2"/>
       <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
-  <dataValidations count="2">
-    <dataValidation type="list" sqref="F2:F3">
-      <formula1>"thùng,bịch,chai,gói,túi,viên,kg,gram,lạng,lít,ml,lọ,bao,cái,cây,điếu"</formula1>
-    </dataValidation>
-    <dataValidation type="list" sqref="J2:J3">
-      <formula1>"Nguyễn Thị Thuỷ(bibica),Nguyễn Đức Cảnh(ĐL cấp 1)"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>